<commit_message>
Add Betting Markets Analytics (Handicap, O/U, BTTS)
</commit_message>
<xml_diff>
--- a/prediction_tracker.xlsx
+++ b/prediction_tracker.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -529,6 +529,21 @@
           <t>Away_Win_Prob</t>
         </is>
       </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Pred_Handicap</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Pred_OU</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Pred_BTTS</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -588,6 +603,9 @@
       <c r="Q2" t="inlineStr"/>
       <c r="R2" t="inlineStr"/>
       <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -661,6 +679,9 @@
       <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr"/>
       <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -734,6 +755,9 @@
       <c r="Q4" t="inlineStr"/>
       <c r="R4" t="inlineStr"/>
       <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -807,6 +831,9 @@
       <c r="Q5" t="inlineStr"/>
       <c r="R5" t="inlineStr"/>
       <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -880,6 +907,9 @@
       <c r="Q6" t="inlineStr"/>
       <c r="R6" t="inlineStr"/>
       <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -953,6 +983,9 @@
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
       <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1026,6 +1059,9 @@
       <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr"/>
       <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1099,6 +1135,9 @@
       <c r="Q9" t="inlineStr"/>
       <c r="R9" t="inlineStr"/>
       <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1172,6 +1211,9 @@
       <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr"/>
       <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1245,6 +1287,9 @@
       <c r="Q11" t="inlineStr"/>
       <c r="R11" t="inlineStr"/>
       <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1318,6 +1363,9 @@
       <c r="Q12" t="inlineStr"/>
       <c r="R12" t="inlineStr"/>
       <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1391,6 +1439,9 @@
       <c r="Q13" t="inlineStr"/>
       <c r="R13" t="inlineStr"/>
       <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1464,6 +1515,9 @@
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
       <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1504,15 +1558,36 @@
           <t>Away</t>
         </is>
       </c>
-      <c r="K15" t="inlineStr"/>
-      <c r="L15" t="inlineStr"/>
-      <c r="M15" t="inlineStr"/>
-      <c r="N15" t="inlineStr"/>
-      <c r="O15" t="inlineStr"/>
-      <c r="P15" t="inlineStr"/>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>0-3</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>Away</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
+        <v>1</v>
+      </c>
+      <c r="N15" t="n">
+        <v>0</v>
+      </c>
+      <c r="O15" t="n">
+        <v>2</v>
+      </c>
+      <c r="P15" t="inlineStr">
+        <is>
+          <t>Sim v6.0 Correct result. Barcola hat-trick.</t>
+        </is>
+      </c>
       <c r="Q15" t="inlineStr"/>
       <c r="R15" t="inlineStr"/>
       <c r="S15" t="inlineStr"/>
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="inlineStr"/>
+      <c r="V15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1553,15 +1628,36 @@
           <t>Away</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr"/>
-      <c r="L16" t="inlineStr"/>
-      <c r="M16" t="inlineStr"/>
-      <c r="N16" t="inlineStr"/>
-      <c r="O16" t="inlineStr"/>
-      <c r="P16" t="inlineStr"/>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>4-0</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0</v>
+      </c>
+      <c r="O16" t="n">
+        <v>4</v>
+      </c>
+      <c r="P16" t="inlineStr">
+        <is>
+          <t>System failure. Predicted Away/Draw, Actual Home rout.</t>
+        </is>
+      </c>
       <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr"/>
       <c r="S16" t="inlineStr"/>
+      <c r="T16" t="inlineStr"/>
+      <c r="U16" t="inlineStr"/>
+      <c r="V16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1602,15 +1698,476 @@
           <t>Away</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
-      <c r="M17" t="inlineStr"/>
-      <c r="N17" t="inlineStr"/>
-      <c r="O17" t="inlineStr"/>
-      <c r="P17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>1-1</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Draw</t>
+        </is>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0</v>
+      </c>
+      <c r="O17" t="n">
+        <v>2</v>
+      </c>
+      <c r="P17" t="inlineStr">
+        <is>
+          <t>Arsenal dropped points. Late equalizer by Brentford.</t>
+        </is>
+      </c>
       <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr"/>
       <c r="S17" t="inlineStr"/>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>2026-02-12</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Atlético Madrid vs Barcelona</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>La_Liga</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Atlético Madrid</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Barcelona</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>31.58</v>
+      </c>
+      <c r="G18" t="n">
+        <v>22.51</v>
+      </c>
+      <c r="H18" t="n">
+        <v>45.91</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>1-1</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>Away</t>
+        </is>
+      </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>4-0</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+      <c r="N18" t="n">
+        <v>0</v>
+      </c>
+      <c r="O18" t="n">
+        <v>4</v>
+      </c>
+      <c r="P18" t="inlineStr">
+        <is>
+          <t>System failure. Predicted Away/Draw, Actual Home rout.</t>
+        </is>
+      </c>
+      <c r="Q18" t="inlineStr"/>
+      <c r="R18" t="inlineStr"/>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Dortmund vs Mainz</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Dortmund</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Mainz</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>65.5</v>
+      </c>
+      <c r="G19" t="n">
+        <v>20</v>
+      </c>
+      <c r="H19" t="n">
+        <v>14.5</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>3-1</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>4-0</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="M19" t="n">
+        <v>1</v>
+      </c>
+      <c r="N19" t="n">
+        <v>0</v>
+      </c>
+      <c r="O19" t="n">
+        <v>2</v>
+      </c>
+      <c r="P19" t="inlineStr">
+        <is>
+          <t>Guirassy scored 2 goals. Comfortable win as predicted.</t>
+        </is>
+      </c>
+      <c r="Q19" t="inlineStr"/>
+      <c r="R19" t="inlineStr"/>
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>2026-02-13</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Pisa vs Milan</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Serie_A</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Pisa</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Milan</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>22.5</v>
+      </c>
+      <c r="G20" t="n">
+        <v>23.15</v>
+      </c>
+      <c r="H20" t="n">
+        <v>54.35</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>0-1</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>Away</t>
+        </is>
+      </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>1-2</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Away</t>
+        </is>
+      </c>
+      <c r="M20" t="n">
+        <v>1</v>
+      </c>
+      <c r="N20" t="n">
+        <v>0</v>
+      </c>
+      <c r="O20" t="n">
+        <v>0</v>
+      </c>
+      <c r="P20" t="inlineStr">
+        <is>
+          <t>Correct Result &amp; Goal Diff. Milan won 2-1 (Modric winner).</t>
+        </is>
+      </c>
+      <c r="Q20" t="inlineStr"/>
+      <c r="R20" t="inlineStr"/>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" t="inlineStr"/>
+      <c r="V20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2026-02-14</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Leverkusen vs St. Pauli</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Leverkusen</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>St. Pauli</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>60.2</v>
+      </c>
+      <c r="G21" t="n">
+        <v>19.73</v>
+      </c>
+      <c r="H21" t="n">
+        <v>20.07</v>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>2-1</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>4-0</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="M21" t="n">
+        <v>1</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0</v>
+      </c>
+      <c r="O21" t="n">
+        <v>3</v>
+      </c>
+      <c r="P21" t="inlineStr">
+        <is>
+          <t>Correct Result. Leverkusen dominant win (4-0).</t>
+        </is>
+      </c>
+      <c r="Q21" t="inlineStr"/>
+      <c r="R21" t="inlineStr"/>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr"/>
+      <c r="V21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2026-02-15</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Leverkusen vs St. Pauli</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Bundesliga</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Leverkusen</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>St. Pauli</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>59.41</v>
+      </c>
+      <c r="G22" t="n">
+        <v>20.45</v>
+      </c>
+      <c r="H22" t="n">
+        <v>20.14</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>2-1</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
+      <c r="Q22" t="inlineStr"/>
+      <c r="R22" t="inlineStr"/>
+      <c r="S22" t="inlineStr"/>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>{'Home -1.5': 36.24, 'Home -0.5': 59.41, 'Home 0.5': 79.86, 'Home 1.5': 92.55}</t>
+        </is>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>{'Over 1.5': 82.65, 'Over 2.5': 61.46, 'Over 3.5': 39.42}</t>
+        </is>
+      </c>
+      <c r="V22" t="n">
+        <v>59.09</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2026-02-15</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Inter vs Juventus</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Serie_A</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Inter</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Juventus</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>45.57</v>
+      </c>
+      <c r="G23" t="n">
+        <v>23.95</v>
+      </c>
+      <c r="H23" t="n">
+        <v>30.48</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>1-1</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
+      <c r="Q23" t="inlineStr"/>
+      <c r="R23" t="inlineStr"/>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>{'Home -1.5': 23.1, 'Home -0.5': 45.57, 'Home 0.5': 69.52000000000001, 'Home 1.5': 87.66000000000001}</t>
+        </is>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>{'Over 1.5': 77.66, 'Over 2.5': 54.67999999999999, 'Over 3.5': 32.45}</t>
+        </is>
+      </c>
+      <c r="V23" t="n">
+        <v>57.06</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Merge 73949dc and restore local changes
</commit_message>
<xml_diff>
--- a/prediction_tracker.xlsx
+++ b/prediction_tracker.xlsx
@@ -12,9 +12,6 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bet data" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bet predic" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="bet ev" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model Eval" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model Eval League" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Model Eval Segments" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -432,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC30"/>
+  <dimension ref="A1:X29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -561,31 +558,6 @@
           <t>Context_Header</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t>Expected_Goals_Home</t>
-        </is>
-      </c>
-      <c r="Z1" s="1" t="inlineStr">
-        <is>
-          <t>Expected_Goals_Away</t>
-        </is>
-      </c>
-      <c r="AA1" s="1" t="inlineStr">
-        <is>
-          <t>Base_Expected_Goals_Home</t>
-        </is>
-      </c>
-      <c r="AB1" s="1" t="inlineStr">
-        <is>
-          <t>Base_Expected_Goals_Away</t>
-        </is>
-      </c>
-      <c r="AC1" s="1" t="inlineStr">
-        <is>
-          <t>Target_Score_Input</t>
-        </is>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -664,11 +636,6 @@
       <c r="V2" t="inlineStr"/>
       <c r="W2" t="inlineStr"/>
       <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
-      <c r="Z2" t="inlineStr"/>
-      <c r="AA2" t="inlineStr"/>
-      <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -747,11 +714,6 @@
       <c r="V3" t="inlineStr"/>
       <c r="W3" t="inlineStr"/>
       <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
-      <c r="Z3" t="inlineStr"/>
-      <c r="AA3" t="inlineStr"/>
-      <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -830,11 +792,6 @@
       <c r="V4" t="inlineStr"/>
       <c r="W4" t="inlineStr"/>
       <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
-      <c r="Z4" t="inlineStr"/>
-      <c r="AA4" t="inlineStr"/>
-      <c r="AB4" t="inlineStr"/>
-      <c r="AC4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -913,11 +870,6 @@
       <c r="V5" t="inlineStr"/>
       <c r="W5" t="inlineStr"/>
       <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr"/>
-      <c r="Z5" t="inlineStr"/>
-      <c r="AA5" t="inlineStr"/>
-      <c r="AB5" t="inlineStr"/>
-      <c r="AC5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -996,11 +948,6 @@
       <c r="V6" t="inlineStr"/>
       <c r="W6" t="inlineStr"/>
       <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
-      <c r="Z6" t="inlineStr"/>
-      <c r="AA6" t="inlineStr"/>
-      <c r="AB6" t="inlineStr"/>
-      <c r="AC6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1079,11 +1026,6 @@
       <c r="V7" t="inlineStr"/>
       <c r="W7" t="inlineStr"/>
       <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
-      <c r="Z7" t="inlineStr"/>
-      <c r="AA7" t="inlineStr"/>
-      <c r="AB7" t="inlineStr"/>
-      <c r="AC7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1162,11 +1104,6 @@
       <c r="V8" t="inlineStr"/>
       <c r="W8" t="inlineStr"/>
       <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
-      <c r="Z8" t="inlineStr"/>
-      <c r="AA8" t="inlineStr"/>
-      <c r="AB8" t="inlineStr"/>
-      <c r="AC8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1245,11 +1182,6 @@
       <c r="V9" t="inlineStr"/>
       <c r="W9" t="inlineStr"/>
       <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
-      <c r="Z9" t="inlineStr"/>
-      <c r="AA9" t="inlineStr"/>
-      <c r="AB9" t="inlineStr"/>
-      <c r="AC9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1328,11 +1260,6 @@
       <c r="V10" t="inlineStr"/>
       <c r="W10" t="inlineStr"/>
       <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
-      <c r="Z10" t="inlineStr"/>
-      <c r="AA10" t="inlineStr"/>
-      <c r="AB10" t="inlineStr"/>
-      <c r="AC10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1411,11 +1338,6 @@
       <c r="V11" t="inlineStr"/>
       <c r="W11" t="inlineStr"/>
       <c r="X11" t="inlineStr"/>
-      <c r="Y11" t="inlineStr"/>
-      <c r="Z11" t="inlineStr"/>
-      <c r="AA11" t="inlineStr"/>
-      <c r="AB11" t="inlineStr"/>
-      <c r="AC11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1494,11 +1416,6 @@
       <c r="V12" t="inlineStr"/>
       <c r="W12" t="inlineStr"/>
       <c r="X12" t="inlineStr"/>
-      <c r="Y12" t="inlineStr"/>
-      <c r="Z12" t="inlineStr"/>
-      <c r="AA12" t="inlineStr"/>
-      <c r="AB12" t="inlineStr"/>
-      <c r="AC12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1577,11 +1494,6 @@
       <c r="V13" t="inlineStr"/>
       <c r="W13" t="inlineStr"/>
       <c r="X13" t="inlineStr"/>
-      <c r="Y13" t="inlineStr"/>
-      <c r="Z13" t="inlineStr"/>
-      <c r="AA13" t="inlineStr"/>
-      <c r="AB13" t="inlineStr"/>
-      <c r="AC13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1660,11 +1572,6 @@
       <c r="V14" t="inlineStr"/>
       <c r="W14" t="inlineStr"/>
       <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr"/>
-      <c r="Z14" t="inlineStr"/>
-      <c r="AA14" t="inlineStr"/>
-      <c r="AB14" t="inlineStr"/>
-      <c r="AC14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1743,11 +1650,6 @@
       <c r="V15" t="inlineStr"/>
       <c r="W15" t="inlineStr"/>
       <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="inlineStr"/>
-      <c r="Z15" t="inlineStr"/>
-      <c r="AA15" t="inlineStr"/>
-      <c r="AB15" t="inlineStr"/>
-      <c r="AC15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1826,11 +1728,6 @@
       <c r="V16" t="inlineStr"/>
       <c r="W16" t="inlineStr"/>
       <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="inlineStr"/>
-      <c r="Z16" t="inlineStr"/>
-      <c r="AA16" t="inlineStr"/>
-      <c r="AB16" t="inlineStr"/>
-      <c r="AC16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1909,11 +1806,6 @@
       <c r="V17" t="inlineStr"/>
       <c r="W17" t="inlineStr"/>
       <c r="X17" t="inlineStr"/>
-      <c r="Y17" t="inlineStr"/>
-      <c r="Z17" t="inlineStr"/>
-      <c r="AA17" t="inlineStr"/>
-      <c r="AB17" t="inlineStr"/>
-      <c r="AC17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1992,11 +1884,6 @@
       <c r="V18" t="inlineStr"/>
       <c r="W18" t="inlineStr"/>
       <c r="X18" t="inlineStr"/>
-      <c r="Y18" t="inlineStr"/>
-      <c r="Z18" t="inlineStr"/>
-      <c r="AA18" t="inlineStr"/>
-      <c r="AB18" t="inlineStr"/>
-      <c r="AC18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2075,11 +1962,6 @@
       <c r="V19" t="inlineStr"/>
       <c r="W19" t="inlineStr"/>
       <c r="X19" t="inlineStr"/>
-      <c r="Y19" t="inlineStr"/>
-      <c r="Z19" t="inlineStr"/>
-      <c r="AA19" t="inlineStr"/>
-      <c r="AB19" t="inlineStr"/>
-      <c r="AC19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2140,11 +2022,6 @@
       <c r="V20" t="inlineStr"/>
       <c r="W20" t="inlineStr"/>
       <c r="X20" t="inlineStr"/>
-      <c r="Y20" t="inlineStr"/>
-      <c r="Z20" t="inlineStr"/>
-      <c r="AA20" t="inlineStr"/>
-      <c r="AB20" t="inlineStr"/>
-      <c r="AC20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2205,11 +2082,6 @@
       <c r="V21" t="inlineStr"/>
       <c r="W21" t="inlineStr"/>
       <c r="X21" t="inlineStr"/>
-      <c r="Y21" t="inlineStr"/>
-      <c r="Z21" t="inlineStr"/>
-      <c r="AA21" t="inlineStr"/>
-      <c r="AB21" t="inlineStr"/>
-      <c r="AC21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2270,11 +2142,6 @@
       <c r="V22" t="inlineStr"/>
       <c r="W22" t="inlineStr"/>
       <c r="X22" t="inlineStr"/>
-      <c r="Y22" t="inlineStr"/>
-      <c r="Z22" t="inlineStr"/>
-      <c r="AA22" t="inlineStr"/>
-      <c r="AB22" t="inlineStr"/>
-      <c r="AC22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2335,11 +2202,6 @@
       <c r="V23" t="inlineStr"/>
       <c r="W23" t="inlineStr"/>
       <c r="X23" t="inlineStr"/>
-      <c r="Y23" t="inlineStr"/>
-      <c r="Z23" t="inlineStr"/>
-      <c r="AA23" t="inlineStr"/>
-      <c r="AB23" t="inlineStr"/>
-      <c r="AC23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2386,8 +2248,16 @@
           <t>Home</t>
         </is>
       </c>
-      <c r="K24" t="inlineStr"/>
-      <c r="L24" t="inlineStr"/>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>2-0</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
       <c r="M24" t="inlineStr"/>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr"/>
@@ -2400,11 +2270,6 @@
       <c r="V24" t="inlineStr"/>
       <c r="W24" t="inlineStr"/>
       <c r="X24" t="inlineStr"/>
-      <c r="Y24" t="inlineStr"/>
-      <c r="Z24" t="inlineStr"/>
-      <c r="AA24" t="inlineStr"/>
-      <c r="AB24" t="inlineStr"/>
-      <c r="AC24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2465,11 +2330,6 @@
       <c r="V25" t="inlineStr"/>
       <c r="W25" t="inlineStr"/>
       <c r="X25" t="inlineStr"/>
-      <c r="Y25" t="inlineStr"/>
-      <c r="Z25" t="inlineStr"/>
-      <c r="AA25" t="inlineStr"/>
-      <c r="AB25" t="inlineStr"/>
-      <c r="AC25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2516,8 +2376,16 @@
           <t>Away</t>
         </is>
       </c>
-      <c r="K26" t="inlineStr"/>
-      <c r="L26" t="inlineStr"/>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>2-1</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
       <c r="M26" t="inlineStr"/>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
@@ -2558,11 +2426,6 @@
           <t>match=Girona vs Barcelona; date=2026-02-16; league=La Liga</t>
         </is>
       </c>
-      <c r="Y26" t="inlineStr"/>
-      <c r="Z26" t="inlineStr"/>
-      <c r="AA26" t="inlineStr"/>
-      <c r="AB26" t="inlineStr"/>
-      <c r="AC26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2609,8 +2472,16 @@
           <t>Home</t>
         </is>
       </c>
-      <c r="K27" t="inlineStr"/>
-      <c r="L27" t="inlineStr"/>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>0-2</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>Away</t>
+        </is>
+      </c>
       <c r="M27" t="inlineStr"/>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr"/>
@@ -2655,11 +2526,6 @@
           <t>match=Cagliari vs Lecce; date=2026-02-16; league=SerieA</t>
         </is>
       </c>
-      <c r="Y27" t="inlineStr"/>
-      <c r="Z27" t="inlineStr"/>
-      <c r="AA27" t="inlineStr"/>
-      <c r="AB27" t="inlineStr"/>
-      <c r="AC27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2706,30 +2572,12 @@
           <t>Away</t>
         </is>
       </c>
-      <c r="K28" t="inlineStr">
-        <is>
-          <t>2-3</t>
-        </is>
-      </c>
-      <c r="L28" t="inlineStr">
-        <is>
-          <t>Away</t>
-        </is>
-      </c>
-      <c r="M28" t="n">
-        <v>1</v>
-      </c>
-      <c r="N28" t="n">
-        <v>0</v>
-      </c>
-      <c r="O28" t="n">
-        <v>0</v>
-      </c>
-      <c r="P28" t="inlineStr">
-        <is>
-          <t>Actual updated from user: 2-3</t>
-        </is>
-      </c>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
       <c r="Q28" t="inlineStr">
         <is>
           <t>AS Monaco vs Paris Saint-Germain</t>
@@ -2762,46 +2610,41 @@
       </c>
       <c r="W28" t="inlineStr"/>
       <c r="X28" t="inlineStr"/>
-      <c r="Y28" t="inlineStr"/>
-      <c r="Z28" t="inlineStr"/>
-      <c r="AA28" t="inlineStr"/>
-      <c r="AB28" t="inlineStr"/>
-      <c r="AC28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>2026-02-18</t>
+          <t>2026-02-17</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Cagliari vs Lecce</t>
+          <t>Borussia Dortmund vs Atalanta</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Serie_A</t>
+          <t>Champions_League</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Cagliari</t>
+          <t>Borussia Dortmund</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Lecce</t>
+          <t>Atalanta</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>41.17915249871762</v>
+        <v>37.87482918330498</v>
       </c>
       <c r="G29" t="n">
-        <v>29.43379902610466</v>
+        <v>29.19433780269773</v>
       </c>
       <c r="H29" t="n">
-        <v>29.38704847517772</v>
+        <v>32.93083301399729</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -2821,17 +2664,17 @@
       <c r="P29" t="inlineStr"/>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>Cagliari vs Lecce</t>
+          <t>Borussia Dortmund vs Atalanta</t>
         </is>
       </c>
       <c r="R29" t="inlineStr">
         <is>
-          <t>Cagliari</t>
+          <t>Borussia Dortmund</t>
         </is>
       </c>
       <c r="S29" t="inlineStr">
         <is>
-          <t>Lecce</t>
+          <t>Atalanta</t>
         </is>
       </c>
       <c r="T29" t="inlineStr">
@@ -2851,136 +2694,14 @@
       </c>
       <c r="W29" t="inlineStr">
         <is>
-          <t>Context league header 'SerieA' differs from detected league 'Serie_A'.</t>
+          <t>League mismatch from datasets: home=Bundesliga, away=Serie_A. Using 'Champions_League'.</t>
         </is>
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>match=Cagliari vs Lecce; date=2026-02-16; league=SerieA</t>
-        </is>
-      </c>
-      <c r="Y29" t="n">
-        <v>1.341374109890173</v>
-      </c>
-      <c r="Z29" t="n">
-        <v>1.096014906081618</v>
-      </c>
-      <c r="AA29" t="n">
-        <v>1.2416</v>
-      </c>
-      <c r="AB29" t="n">
-        <v>1.145</v>
-      </c>
-      <c r="AC29" t="inlineStr">
-        <is>
-          <t>0-2</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>2026-02-18</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>AS Monaco vs Paris Saint-Germain</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>Ligue_1</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>AS Monaco</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
-          <t>Paris Saint-Germain</t>
-        </is>
-      </c>
-      <c r="F30" t="n">
-        <v>31.57268350351948</v>
-      </c>
-      <c r="G30" t="n">
-        <v>27.55222316894729</v>
-      </c>
-      <c r="H30" t="n">
-        <v>40.87509332753321</v>
-      </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>0-1</t>
-        </is>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>Away</t>
-        </is>
-      </c>
-      <c r="K30" t="inlineStr"/>
-      <c r="L30" t="inlineStr"/>
-      <c r="M30" t="inlineStr"/>
-      <c r="N30" t="inlineStr"/>
-      <c r="O30" t="inlineStr"/>
-      <c r="P30" t="inlineStr"/>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>AS Monaco vs Paris Saint-Germain</t>
-        </is>
-      </c>
-      <c r="R30" t="inlineStr">
-        <is>
-          <t>AS Monaco</t>
-        </is>
-      </c>
-      <c r="S30" t="inlineStr">
-        <is>
-          <t>Paris Saint-Germain</t>
-        </is>
-      </c>
-      <c r="T30" t="inlineStr">
-        <is>
-          <t>1-1</t>
-        </is>
-      </c>
-      <c r="U30" t="inlineStr">
-        <is>
-          <t>Away</t>
-        </is>
-      </c>
-      <c r="V30" t="inlineStr">
-        <is>
-          <t>Away</t>
-        </is>
-      </c>
-      <c r="W30" t="inlineStr">
-        <is>
-          <t>Context match header 'Cagliari vs Lecce' does not match requested fixture 'AS Monaco vs Paris Saint-Germain'. | Context league header 'SerieA' differs from detected league 'Ligue_1'.</t>
-        </is>
-      </c>
-      <c r="X30" t="inlineStr">
-        <is>
-          <t>match=Cagliari vs Lecce; date=2026-02-16; league=SerieA</t>
-        </is>
-      </c>
-      <c r="Y30" t="n">
-        <v>1.276678604934378</v>
-      </c>
-      <c r="Z30" t="n">
-        <v>1.480749154555034</v>
-      </c>
-      <c r="AA30" t="n">
-        <v>1.2395</v>
-      </c>
-      <c r="AB30" t="n">
-        <v>1.5188</v>
-      </c>
-      <c r="AC30" t="inlineStr"/>
+          <t>match=Borussia Dortmund vs Atalanta; date=2026-02-17; league=Champions_League</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3020,7 +2741,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3">
@@ -3030,7 +2751,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4">
@@ -3040,7 +2761,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>63.16</v>
+        <v>52.38</v>
       </c>
     </row>
     <row r="5">
@@ -3060,7 +2781,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>21.05</v>
+        <v>19.05</v>
       </c>
     </row>
     <row r="7">
@@ -3070,7 +2791,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1.42</v>
+        <v>1.5</v>
       </c>
     </row>
   </sheetData>
@@ -3084,7 +2805,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R12"/>
+  <dimension ref="A1:R11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3745,125 +3466,63 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-02-18</t>
+          <t>2026-02-17</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Cagliari vs Lecce</t>
+          <t>Borussia Dortmund vs Atalanta</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Serie_A</t>
+          <t>Champions_League</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>2.1</v>
+        <v>1.8</v>
       </c>
       <c r="E11" t="n">
-        <v>7.1</v>
+        <v>6.3</v>
       </c>
       <c r="F11" t="n">
-        <v>19.6</v>
+        <v>17.7</v>
       </c>
       <c r="G11" t="n">
-        <v>42.3</v>
+        <v>39.1</v>
       </c>
       <c r="H11" t="n">
-        <v>69.5</v>
+        <v>65.90000000000001</v>
       </c>
       <c r="I11" t="n">
-        <v>88</v>
+        <v>85.59999999999999</v>
       </c>
       <c r="J11" t="n">
-        <v>96.40000000000001</v>
+        <v>95.3</v>
       </c>
       <c r="K11" t="n">
-        <v>91.3</v>
+        <v>92</v>
       </c>
       <c r="L11" t="n">
-        <v>8.699999999999999</v>
+        <v>8</v>
       </c>
       <c r="M11" t="n">
-        <v>70</v>
+        <v>71.90000000000001</v>
       </c>
       <c r="N11" t="n">
-        <v>30</v>
+        <v>28.1</v>
       </c>
       <c r="O11" t="n">
-        <v>44</v>
+        <v>46.4</v>
       </c>
       <c r="P11" t="n">
-        <v>56</v>
+        <v>53.6</v>
       </c>
       <c r="Q11" t="n">
-        <v>22.9</v>
+        <v>24.9</v>
       </c>
       <c r="R11" t="n">
-        <v>77.09999999999999</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2026-02-18</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>AS Monaco vs Paris Saint-Germain</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Ligue_1</t>
-        </is>
-      </c>
-      <c r="D12" t="n">
-        <v>1.3</v>
-      </c>
-      <c r="E12" t="n">
-        <v>4.8</v>
-      </c>
-      <c r="F12" t="n">
-        <v>14.1</v>
-      </c>
-      <c r="G12" t="n">
-        <v>32.7</v>
-      </c>
-      <c r="H12" t="n">
-        <v>58</v>
-      </c>
-      <c r="I12" t="n">
-        <v>79.59999999999999</v>
-      </c>
-      <c r="J12" t="n">
-        <v>92.09999999999999</v>
-      </c>
-      <c r="K12" t="n">
-        <v>93.7</v>
-      </c>
-      <c r="L12" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="M12" t="n">
-        <v>76.2</v>
-      </c>
-      <c r="N12" t="n">
-        <v>23.8</v>
-      </c>
-      <c r="O12" t="n">
-        <v>52</v>
-      </c>
-      <c r="P12" t="n">
-        <v>48</v>
-      </c>
-      <c r="Q12" t="n">
-        <v>29.9</v>
-      </c>
-      <c r="R12" t="n">
-        <v>70.09999999999999</v>
+        <v>75.09999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -3877,7 +3536,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4118,8 +3777,16 @@
           <t>Model probability: 85.3%.</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2-0</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Won</t>
+        </is>
+      </c>
       <c r="H6" t="inlineStr"/>
       <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr"/>
@@ -4188,8 +3855,16 @@
           <t>Model-only selection by highest probability 0.753.</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr"/>
-      <c r="G8" t="inlineStr"/>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>2-1</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Won</t>
+        </is>
+      </c>
       <c r="H8" t="inlineStr"/>
       <c r="I8" t="inlineStr"/>
       <c r="J8" t="n">
@@ -4229,8 +3904,16 @@
           <t>Model-only selection by highest probability 0.849.</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>0-2</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Lost</t>
+        </is>
+      </c>
       <c r="H9" t="inlineStr"/>
       <c r="I9" t="inlineStr"/>
       <c r="J9" t="n">
@@ -4270,16 +3953,8 @@
           <t>Model-only selection by highest probability 0.734.</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>2-3</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>Won</t>
-        </is>
-      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr"/>
       <c r="H10" t="inlineStr"/>
       <c r="I10" t="inlineStr"/>
       <c r="J10" t="n">
@@ -4296,12 +3971,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>2026-02-18</t>
+          <t>2026-02-17</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Cagliari vs Lecce</t>
+          <t>Borussia Dortmund vs Atalanta</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -4316,7 +3991,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Model-only selection by highest probability 0.853.</t>
+          <t>Model-only selection by highest probability 0.820.</t>
         </is>
       </c>
       <c r="F11" t="inlineStr"/>
@@ -4324,52 +3999,11 @@
       <c r="H11" t="inlineStr"/>
       <c r="I11" t="inlineStr"/>
       <c r="J11" t="n">
-        <v>0.8532</v>
+        <v>0.8204</v>
       </c>
       <c r="K11" t="inlineStr"/>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr">
-        <is>
-          <t>model_only_best_prob</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2026-02-18</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>AS Monaco vs Paris Saint-Germain</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>HDP +1</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>High</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Model-only selection by highest probability 0.740.</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr"/>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="n">
-        <v>0.7398</v>
-      </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
-      <c r="M12" t="inlineStr">
         <is>
           <t>model_only_best_prob</t>
         </is>
@@ -4444,1111 +4078,4 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:F20"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Section</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Metric</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Value</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Threshold</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Current</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Operator</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>overall</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>n_matches</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>19</v>
-      </c>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>overall</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>result_accuracy</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>0.6316000000000001</v>
-      </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>overall</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>brier_1x2</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0.5185</v>
-      </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
-      <c r="F4" t="inlineStr"/>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>overall</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>log_loss_1x2</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>0.9634</v>
-      </c>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
-      <c r="F5" t="inlineStr"/>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>overall</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>exact_score_accuracy</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>0.2105</v>
-      </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>overall</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>score_mae</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>0.9211</v>
-      </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>overall</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>goal_diff_mae</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>1.4211</v>
-      </c>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
-      <c r="F8" t="inlineStr"/>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>overall</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>home_goal_mae</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>1.1053</v>
-      </c>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>overall</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>away_goal_mae</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>0.7368</v>
-      </c>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
-      <c r="F10" t="inlineStr"/>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>overall</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>total_goals_mae</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>1.1053</v>
-      </c>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
-      <c r="F11" t="inlineStr"/>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>overall</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>xg_mae</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr"/>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>overall</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>xg_rows</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>quality_gate</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>min_completed_matches</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>fail</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>30</v>
-      </c>
-      <c r="E14" t="n">
-        <v>19</v>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>&gt;=</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>quality_gate</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>result_accuracy</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.6316000000000001</v>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>&gt;=</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>quality_gate</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>brier_1x2</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>0.62</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.5185</v>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>&lt;=</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>quality_gate</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>log_loss_1x2</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>1.05</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.9634</v>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>&lt;=</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>quality_gate</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>score_mae</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>pass</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>1.35</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.9211</v>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>&lt;=</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>quality_gate</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>xg_mae</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>insufficient_data</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>0.95</v>
-      </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>&lt;=</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>quality_gate</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>overall_passed</t>
-        </is>
-      </c>
-      <c r="C20" t="b">
-        <v>0</v>
-      </c>
-      <c r="D20" t="inlineStr"/>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:M6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>League</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>n_matches</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>result_accuracy</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>brier_1x2</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>log_loss_1x2</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>exact_score_accuracy</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>score_mae</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>goal_diff_mae</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>home_goal_mae</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>away_goal_mae</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>total_goals_mae</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>xg_mae</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>xg_rows</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Premier_League</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>8</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.6937</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1.3144</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.375</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="H2" t="n">
-        <v>1</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L2" t="inlineStr"/>
-      <c r="M2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Serie_A</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>4</v>
-      </c>
-      <c r="C3" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.379</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.6753</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" t="n">
-        <v>1.125</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="I3" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="J3" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" t="n">
-        <v>2.25</v>
-      </c>
-      <c r="L3" t="inlineStr"/>
-      <c r="M3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Ligue_1</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>3</v>
-      </c>
-      <c r="C4" t="n">
-        <v>0.6667</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0.4424</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0.7803</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="H4" t="n">
-        <v>2.3333</v>
-      </c>
-      <c r="I4" t="n">
-        <v>2</v>
-      </c>
-      <c r="J4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1.6667</v>
-      </c>
-      <c r="L4" t="inlineStr"/>
-      <c r="M4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>La_Liga</t>
-        </is>
-      </c>
-      <c r="B5" t="n">
-        <v>2</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.5214</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.9085</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" t="inlineStr"/>
-      <c r="M5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Bundesliga</t>
-        </is>
-      </c>
-      <c r="B6" t="n">
-        <v>2</v>
-      </c>
-      <c r="C6" t="n">
-        <v>1</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.2081</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.4653</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="H6" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="I6" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:N7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>Segment_Type</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Segment</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>n_matches</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>result_accuracy</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>brier_1x2</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>log_loss_1x2</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>exact_score_accuracy</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>score_mae</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>goal_diff_mae</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>home_goal_mae</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>away_goal_mae</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>total_goals_mae</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>xg_mae</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>xg_rows</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>actual_result</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Away</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>9</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0.8889</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0.3146</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0.6049</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.4444</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.4444</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.4444</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.5556</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.3333</v>
-      </c>
-      <c r="L2" t="n">
-        <v>0.6667</v>
-      </c>
-      <c r="M2" t="inlineStr"/>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>actual_result</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Home</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>6</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0.6667</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0.393</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0.7127</v>
-      </c>
-      <c r="G3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="I3" t="n">
-        <v>2.6667</v>
-      </c>
-      <c r="J3" t="n">
-        <v>2.1667</v>
-      </c>
-      <c r="K3" t="n">
-        <v>0.8333</v>
-      </c>
-      <c r="L3" t="n">
-        <v>1.6667</v>
-      </c>
-      <c r="M3" t="inlineStr"/>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>actual_result</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Draw</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>4</v>
-      </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1.1655</v>
-      </c>
-      <c r="F4" t="n">
-        <v>2.1464</v>
-      </c>
-      <c r="G4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" t="n">
-        <v>1.125</v>
-      </c>
-      <c r="I4" t="n">
-        <v>1.75</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="K4" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="L4" t="n">
-        <v>1.25</v>
-      </c>
-      <c r="M4" t="inlineStr"/>
-      <c r="N4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>pred_result</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Away</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>11</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0.7272999999999999</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0.5278</v>
-      </c>
-      <c r="F5" t="n">
-        <v>1.0313</v>
-      </c>
-      <c r="G5" t="n">
-        <v>0.3636</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.7272999999999999</v>
-      </c>
-      <c r="I5" t="n">
-        <v>1.0909</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.8182</v>
-      </c>
-      <c r="K5" t="n">
-        <v>0.6364</v>
-      </c>
-      <c r="L5" t="n">
-        <v>0.7272999999999999</v>
-      </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>pred_result</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Home</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>6</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0.6667</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0.4746</v>
-      </c>
-      <c r="F6" t="n">
-        <v>0.8277</v>
-      </c>
-      <c r="G6" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" t="n">
-        <v>1.0833</v>
-      </c>
-      <c r="I6" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="J6" t="n">
-        <v>1.1667</v>
-      </c>
-      <c r="K6" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>pred_result</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Draw</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>2</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0.5992</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.9976</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>1.5</v>
-      </c>
-      <c r="I7" t="n">
-        <v>3</v>
-      </c>
-      <c r="J7" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="L7" t="n">
-        <v>2</v>
-      </c>
-      <c r="M7" t="inlineStr"/>
-      <c r="N7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>